<commit_message>
initial commit of in-progress script for analysis of top candidate meteorites
</commit_message>
<xml_diff>
--- a/Candidate Meteorite Details.xlsx
+++ b/Candidate Meteorite Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bureauveritas-my.sharepoint.com/personal/joshua_stuckey_bureauveritas_com/Documents/Documents/Python/Projects/Mjolnir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC104879D11961DA5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{525111A4-4178-4735-B078-0064A1A9BBFD}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_F25DC773A252ABDACC104879D11961DA5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C182CBD7-B5E4-4682-8F3A-420D9FAA922A}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="9700" yWindow="340" windowWidth="9320" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Meteorite Name</t>
   </si>
@@ -33,9 +33,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Date or Date Range</t>
-  </si>
-  <si>
     <t>Denver</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=10842</t>
   </si>
   <si>
-    <t>07/10/1967-07/17/1967</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -109,16 +103,66 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=11202</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=11203</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=22740</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=14716</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=23728</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=373</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=10916</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=16635</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=47355</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=50909</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=23976</t>
+  </si>
+  <si>
+    <t>https://www.lpi.usra.edu/meteor/metbull.cfm?code=23905</t>
+  </si>
+  <si>
+    <t>N/A\</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,13 +185,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -161,6 +209,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,15 +481,15 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -445,132 +497,258 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="1">
+        <v>24670</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1">
+        <v>28156</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1">
+        <v>27176</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1">
+        <v>33948</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1">
+        <v>38265</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1">
+        <v>39470</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1">
+        <v>37458</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>17</v>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{70FBCA58-13C5-427E-B441-67F7049811EA}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{C545B5BB-9F11-4B1D-9AAD-5982A364C884}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{59BCECE1-F087-483D-BE1C-5B46C077B37F}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{2323E8AE-A213-46E1-A43C-4607F46EBDFB}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{C32DA5A0-2FF5-4A74-948B-2693E3AA8D38}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{2EA45FEE-9D1E-42EB-83FE-9AE838F4AB26}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{D4BA5923-BE29-4FF2-8ECE-36B908CB13DD}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{56712A3F-1CE6-4172-9242-D3B14DBA6A63}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{CEB1282D-900F-4FA5-84FB-6AC71DB27122}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{78A43B7E-FB09-4235-9F51-BE890FCBA230}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{9124D766-DA5B-4BC6-8577-A2D98BBEBF48}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{60F26140-644F-44BF-84FF-925556B838EB}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{C014E29A-0BF2-4756-AB67-FC7CE8D6436D}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{5869E900-0800-42A5-B4B3-750662E8F7D7}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{153458BF-D272-4D76-A426-0E7F35A8474E}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{7879819E-AB5D-4C55-BC10-F540437738BE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
setup for portfolio-ready refactor: requirements.txt, README initial rewrite, etc.
</commit_message>
<xml_diff>
--- a/Candidate Meteorite Details.xlsx
+++ b/Candidate Meteorite Details.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="118" documentId="11_F25DC773A252ABDACC104879D11961DA5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C182CBD7-B5E4-4682-8F3A-420D9FAA922A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="9700" yWindow="340" windowWidth="9320" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>